<commit_message>
Updated .rmd files and .tex and .pdf from 30th June, after synchronising LateX and bookdown files.
</commit_message>
<xml_diff>
--- a/publisher bits/Artwork+and+third-party+material+permissions+log.xlsx
+++ b/publisher bits/Artwork+and+third-party+material+permissions+log.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorothybishop/Rprojects/EvaluatingWhatWorks2023/publisher bits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6708E3F8-1BF5-A841-86DF-043D993A89FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D8175A-E967-0145-8AC0-ECC30BC25A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20000" yWindow="9420" windowWidth="18580" windowHeight="11200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20000" yWindow="9420" windowWidth="18580" windowHeight="11200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Image log" sheetId="1" r:id="rId1"/>
-    <sheet name="Table log" sheetId="5" r:id="rId2"/>
-    <sheet name="Boxes" sheetId="3" r:id="rId3"/>
-    <sheet name="Instructions for use" sheetId="2" r:id="rId4"/>
+    <sheet name="formatting bits" sheetId="7" r:id="rId2"/>
+    <sheet name="Table log" sheetId="5" r:id="rId3"/>
+    <sheet name="html" sheetId="6" r:id="rId4"/>
+    <sheet name="Boxes" sheetId="3" r:id="rId5"/>
+    <sheet name="Instructions for use" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="425">
   <si>
     <t>Type</t>
   </si>
@@ -1221,6 +1223,96 @@
   </si>
   <si>
     <t>tab: singlecasechart</t>
+  </si>
+  <si>
+    <t>[Statistical Thinking for the 21st Century](https://github.com/statsthinking21/statsthinking21)</t>
+  </si>
+  <si>
+    <t>chapter</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>Preface</t>
+  </si>
+  <si>
+    <t>ix</t>
+  </si>
+  <si>
+    <t>[ModernDive: Statistical Inference via Data Science](https://moderndive.com/)</t>
+  </si>
+  <si>
+    <t>For more explanation see &lt;https://www.measurement-toolkit.org/concepts/statistical-assessment&gt;.</t>
+  </si>
+  <si>
+    <t>REMOVED</t>
+  </si>
+  <si>
+    <t>[Cogmed Working Memory Training](https://www.cogmed.com/)</t>
+  </si>
+  <si>
+    <t>[this blogpost](http://deevybee.blogspot.com/2011/04/short-nerdy-post-about-use-of.html) gives a short explanation.</t>
+  </si>
+  <si>
+    <t>placement</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Fig 3.5 needs to be nearer to text</t>
+  </si>
+  <si>
+    <t>Formatting of text below exercise 2 needs fixing</t>
+  </si>
+  <si>
+    <t>[EasyPeasy](https://guidebook.eif.org.uk/programme/easypeasy)</t>
+  </si>
+  <si>
+    <t>[report by the Education Endowment Foundation](https://d2tic4wvo1iusb.cloudfront.net/documents/projects/EasyPeasy.pdf?v=1686132397)</t>
+  </si>
+  <si>
+    <t>[This website](https://www.andifugard.info/regression-to-the-mean/)</t>
+  </si>
+  <si>
+    <t>[A similar picture was observed in 2013](http://deevybee.blogspot.com/2013/10/good-and-bad-news-on-phonics-screen.html),</t>
+  </si>
+  <si>
+    <t>[this website](https://data.library.virginia.edu/getting-started-with-multiple-imputation-in-r/))</t>
+  </si>
+  <si>
+    <t>[this website](https://www.missingdata.nl/) by Iris Eekhout.</t>
+  </si>
+  <si>
+    <t>[CONSORT website](http://www.consort-statement.org/consort-statement/flow-diagram)</t>
+  </si>
+  <si>
+    <t>registered on a site such as &lt;https://clinicaltrials.gov/&gt;</t>
+  </si>
+  <si>
+    <t>[EQUATOR](http://www.equator-network.org)</t>
+  </si>
+  <si>
+    <t>[This website](https://www.mathsisfun.com/data/standard-deviation.html)</t>
+  </si>
+  <si>
+    <t>Look at this website: https://shiny.rit.albany.edu/stat/confidence/</t>
+  </si>
+  <si>
+    <t>[pirate plot](https://www.psychologicalscience.org/observer/yarrr-the-pirates-guide-to-r)</t>
+  </si>
+  <si>
+    <t>[this website](http://www.sthda.com/english/articles/39-regression-model-diagnostics/161-linear-regression-assumptions-and-diagnostics-in-r-essentials/)</t>
+  </si>
+  <si>
+    <t>[this blogpost by Daniël Lakens](http://daniellakens.blogspot.com/2016/03/one-sided-tests-efficient-and-underused.html).</t>
+  </si>
+  <si>
+    <t>See [this blogpost](http://deevybee.blogspot.com/2017/11/anova-t-tests-and-regression-different.html) for more details.</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1376,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1315,6 +1407,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1338,7 +1436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1369,6 +1467,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1755,42 +1854,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="3" width="67.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="53" style="1" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="44.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.83203125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="17.5" style="1" customWidth="1"/>
-    <col min="13" max="1025" width="8.6640625" style="1" customWidth="1"/>
-    <col min="1026" max="16384" width="8.83203125" style="1"/>
+    <col min="2" max="3" width="8" style="1" customWidth="1"/>
+    <col min="4" max="4" width="67.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="53" style="1" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.83203125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="17.5" style="1" customWidth="1"/>
+    <col min="14" max="1026" width="8.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>54</v>
       </c>
@@ -1798,266 +1898,270 @@
         <v>293</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="49" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="C3"/>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3"/>
+      <c r="E3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B5" s="1">
         <v>233</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>149</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>169</v>
       </c>
@@ -2065,1036 +2169,1041 @@
         <v>148</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>199</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>212</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>221</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>223</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>227</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>235</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>236</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>198</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>240</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>241</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>242</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>243</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>244</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>345</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="D33" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="E33" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="F33" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G33" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="15" t="s">
+      <c r="H33" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>265</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>246</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>247</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>248</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>249</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>270</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>251</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>269</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>252</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>275</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="E41" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>280</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>253</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>281</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>254</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>255</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G45" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I45" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>283</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>256</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>258</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I48" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>284</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>259</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="H49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I49" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>286</v>
       </c>
       <c r="B50" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="13"/>
+      <c r="D50" t="s">
         <v>260</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="3" t="s">
+      <c r="H50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I50" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>288</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="13"/>
+      <c r="D51" t="s">
         <v>261</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="H51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>289</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>292</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>262</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G53" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I53" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>142</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="K54" s="1" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3108,10 +3217,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9940E52B-3371-7E4F-8B0F-2A97F1C99CA4}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4C639D-2DF9-D341-8783-1321FF2F763E}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
@@ -3335,13 +3469,262 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A732829-AC8B-1140-989F-F00EB5FDD460}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="97.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>91</v>
+      </c>
+      <c r="C21" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB99A36-8393-46E6-BB93-19D034D5252B}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3440,15 +3823,18 @@
         <v>309</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="18" t="s">
         <v>310</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3606,7 +3992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70F0744-3404-42E3-A223-085625505051}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -3937,15 +4323,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Updated xmlns="087fd999-e084-461a-80de-38f79316e189" xsi:nil="true"/>
-    <TaxCatchAll xmlns="673dc59d-a9fa-4568-a0b5-e8c44363c7cb" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="087fd999-e084-461a-80de-38f79316e189">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4198,21 +4581,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Updated xmlns="087fd999-e084-461a-80de-38f79316e189" xsi:nil="true"/>
+    <TaxCatchAll xmlns="673dc59d-a9fa-4568-a0b5-e8c44363c7cb" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="087fd999-e084-461a-80de-38f79316e189">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63FF162A-8891-4D08-87CE-1D7BF7B46742}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D56064-A181-4DD5-B8A9-300581D67C4C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="087fd999-e084-461a-80de-38f79316e189"/>
-    <ds:schemaRef ds:uri="673dc59d-a9fa-4568-a0b5-e8c44363c7cb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4237,9 +4620,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D56064-A181-4DD5-B8A9-300581D67C4C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63FF162A-8891-4D08-87CE-1D7BF7B46742}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="087fd999-e084-461a-80de-38f79316e189"/>
+    <ds:schemaRef ds:uri="673dc59d-a9fa-4568-a0b5-e8c44363c7cb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>